<commit_message>
Code modification and documentation update
</commit_message>
<xml_diff>
--- a/devdata/Employee data.xlsx
+++ b/devdata/Employee data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
@@ -30,7 +30,7 @@
     <t>Last name</t>
   </si>
   <si>
-    <t>Pakiraam</t>
+    <t>Funny</t>
   </si>
   <si>
     <t>Date of birth</t>
@@ -64,9 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,13 +76,13 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -162,7 +160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,12 +171,15 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -186,10 +187,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,8 +500,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="27.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="27.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -530,7 +531,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5">
-        <v>25569.12532803241</v>
+        <v>32117</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
@@ -543,39 +544,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
+      <c r="B7" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="B9" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+      <c r="B10" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
+      <c r="B11" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
+      <c r="B12" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
+      <c r="B13" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -592,12 +593,12 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="27.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="27.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -606,7 +607,7 @@
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -614,7 +615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -622,15 +623,15 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5">
-        <v>25569.12535078704</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <v>23056</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -638,41 +639,41 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="B6" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="B7" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="B8" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="B9" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="B10" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="B11" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="B12" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
+      <c r="B13" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -689,12 +690,12 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="27.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="27.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -724,7 +725,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5">
-        <v>25569.125382233797</v>
+        <v>33329</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
@@ -737,39 +738,39 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
+      <c r="B6" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
+      <c r="B7" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
+      <c r="B8" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="B9" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+      <c r="B10" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
+      <c r="B11" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
+      <c r="B12" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
+      <c r="B13" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>